<commit_message>
button download dan update + toastr + new sidebar + eye toogle
</commit_message>
<xml_diff>
--- a/public/storage/simpanFile/daftar_pd-SMP KANISIUS GAYAM YOGYAKARTA-2023-07-13 11_24_36.xlsx
+++ b/public/storage/simpanFile/daftar_pd-SMP KANISIUS GAYAM YOGYAKARTA-2023-07-13 11_24_36.xlsx
@@ -7940,7 +7940,7 @@
       <c r="BM6" s="11"/>
       <c r="BN6" s="11"/>
       <c r="BO6">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="7" spans="1:67">
@@ -8080,7 +8080,7 @@
         <v>2</v>
       </c>
       <c r="BO7">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="8" spans="1:67">
@@ -8241,7 +8241,7 @@
         <v>2</v>
       </c>
       <c r="BO8">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="9" spans="1:67">
@@ -8378,7 +8378,7 @@
         <v>0</v>
       </c>
       <c r="BO9">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="10" spans="1:67">
@@ -8524,7 +8524,7 @@
         <v>4</v>
       </c>
       <c r="BO10">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="11" spans="1:67">
@@ -8670,7 +8670,7 @@
         <v>0</v>
       </c>
       <c r="BO11">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="12" spans="1:67">
@@ -8816,7 +8816,7 @@
         <v>15</v>
       </c>
       <c r="BO12">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="13" spans="1:67">
@@ -8971,7 +8971,7 @@
         <v>1</v>
       </c>
       <c r="BO13">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="14" spans="1:67">
@@ -9114,7 +9114,7 @@
         <v>1</v>
       </c>
       <c r="BO14">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="15" spans="1:67">
@@ -9275,7 +9275,7 @@
         <v>5</v>
       </c>
       <c r="BO15">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="16" spans="1:67">
@@ -9409,7 +9409,7 @@
         <v>2</v>
       </c>
       <c r="BO16">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="17" spans="1:67">
@@ -9567,7 +9567,7 @@
         <v>3</v>
       </c>
       <c r="BO17">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="18" spans="1:67">
@@ -9716,7 +9716,7 @@
         <v>6</v>
       </c>
       <c r="BO18">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="19" spans="1:67">
@@ -9871,7 +9871,7 @@
         <v>1</v>
       </c>
       <c r="BO19">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="20" spans="1:67">
@@ -10005,7 +10005,7 @@
         <v>0</v>
       </c>
       <c r="BO20">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="21" spans="1:67">
@@ -10163,7 +10163,7 @@
         <v>1</v>
       </c>
       <c r="BO21">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="22" spans="1:67">
@@ -10309,7 +10309,7 @@
         <v>5</v>
       </c>
       <c r="BO22">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="23" spans="1:67">
@@ -10458,7 +10458,7 @@
         <v>0</v>
       </c>
       <c r="BO23">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="24" spans="1:67">
@@ -10610,7 +10610,7 @@
         <v>3</v>
       </c>
       <c r="BO24">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="25" spans="1:67">
@@ -10756,7 +10756,7 @@
         <v>1</v>
       </c>
       <c r="BO25">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="26" spans="1:67">
@@ -10905,7 +10905,7 @@
         <v>0</v>
       </c>
       <c r="BO26">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="27" spans="1:67">
@@ -11042,7 +11042,7 @@
         <v>0</v>
       </c>
       <c r="BO27">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="28" spans="1:67">
@@ -11179,7 +11179,7 @@
         <v>8</v>
       </c>
       <c r="BO28">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="29" spans="1:67">
@@ -11322,7 +11322,7 @@
         <v>10</v>
       </c>
       <c r="BO29">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="30" spans="1:67">
@@ -11459,7 +11459,7 @@
         <v>0</v>
       </c>
       <c r="BO30">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="31" spans="1:67">
@@ -11611,7 +11611,7 @@
         <v>1</v>
       </c>
       <c r="BO31">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="32" spans="1:67">
@@ -11736,7 +11736,7 @@
         <v>7</v>
       </c>
       <c r="BO32">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="33" spans="1:67">
@@ -11879,7 +11879,7 @@
         <v>0</v>
       </c>
       <c r="BO33">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="34" spans="1:67">
@@ -12025,7 +12025,7 @@
         <v>1</v>
       </c>
       <c r="BO34">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="35" spans="1:67">
@@ -12174,7 +12174,7 @@
         <v>0</v>
       </c>
       <c r="BO35">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="36" spans="1:67">
@@ -12329,7 +12329,7 @@
         <v>1</v>
       </c>
       <c r="BO36">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="37" spans="1:67">
@@ -12457,7 +12457,7 @@
         <v>1</v>
       </c>
       <c r="BO37">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="38" spans="1:67">
@@ -12612,7 +12612,7 @@
         <v>4</v>
       </c>
       <c r="BO38">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="39" spans="1:67">
@@ -12767,7 +12767,7 @@
         <v>1</v>
       </c>
       <c r="BO39">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="40" spans="1:67">
@@ -12925,7 +12925,7 @@
         <v>3</v>
       </c>
       <c r="BO40">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="41" spans="1:67">
@@ -13065,7 +13065,7 @@
         <v>1</v>
       </c>
       <c r="BO41">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="42" spans="1:67">
@@ -13217,7 +13217,7 @@
         <v>0</v>
       </c>
       <c r="BO42">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="43" spans="1:67">
@@ -13360,7 +13360,7 @@
         <v>0</v>
       </c>
       <c r="BO43">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="44" spans="1:67">
@@ -13476,7 +13476,7 @@
         <v>1</v>
       </c>
       <c r="BO44">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="45" spans="1:67">
@@ -13622,7 +13622,7 @@
         <v>0</v>
       </c>
       <c r="BO45">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="46" spans="1:67">
@@ -13762,7 +13762,7 @@
         <v>0</v>
       </c>
       <c r="BO46">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="47" spans="1:67">
@@ -13896,7 +13896,7 @@
         <v>1</v>
       </c>
       <c r="BO47">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="48" spans="1:67">
@@ -14045,7 +14045,7 @@
         <v>1</v>
       </c>
       <c r="BO48">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="49" spans="1:67">
@@ -14188,7 +14188,7 @@
         <v>0</v>
       </c>
       <c r="BO49">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="50" spans="1:67">
@@ -14313,7 +14313,7 @@
         <v>1</v>
       </c>
       <c r="BO50">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="51" spans="1:67">
@@ -14453,7 +14453,7 @@
         <v>2</v>
       </c>
       <c r="BO51">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="52" spans="1:67">
@@ -14605,7 +14605,7 @@
         <v>1</v>
       </c>
       <c r="BO52">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="53" spans="1:67">
@@ -14748,7 +14748,7 @@
         <v>0</v>
       </c>
       <c r="BO53">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="54" spans="1:67">
@@ -14867,7 +14867,7 @@
         <v>5</v>
       </c>
       <c r="BO54">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="55" spans="1:67">
@@ -15004,7 +15004,7 @@
         <v>4</v>
       </c>
       <c r="BO55">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="56" spans="1:67">
@@ -15153,7 +15153,7 @@
         <v>1</v>
       </c>
       <c r="BO56">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="57" spans="1:67">
@@ -15296,7 +15296,7 @@
         <v>1</v>
       </c>
       <c r="BO57">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="58" spans="1:67">
@@ -15433,7 +15433,7 @@
         <v>1</v>
       </c>
       <c r="BO58">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="59" spans="1:67">
@@ -15585,7 +15585,7 @@
         <v>3</v>
       </c>
       <c r="BO59">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="60" spans="1:67">
@@ -15710,7 +15710,7 @@
         <v>1</v>
       </c>
       <c r="BO60">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="61" spans="1:67">
@@ -15856,7 +15856,7 @@
         <v>0</v>
       </c>
       <c r="BO61">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="62" spans="1:67">
@@ -15984,7 +15984,7 @@
         <v>10</v>
       </c>
       <c r="BO62">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="63" spans="1:67">
@@ -16127,7 +16127,7 @@
         <v>1</v>
       </c>
       <c r="BO63">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="64" spans="1:67">
@@ -16276,7 +16276,7 @@
         <v>1</v>
       </c>
       <c r="BO64">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="65" spans="1:67">
@@ -16419,7 +16419,7 @@
         <v>1</v>
       </c>
       <c r="BO65">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="66" spans="1:67">
@@ -16550,7 +16550,7 @@
         <v>1</v>
       </c>
       <c r="BO66">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="67" spans="1:67">
@@ -16693,7 +16693,7 @@
         <v>3</v>
       </c>
       <c r="BO67">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="68" spans="1:67">
@@ -16839,7 +16839,7 @@
         <v>2</v>
       </c>
       <c r="BO68">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="69" spans="1:67">
@@ -16988,7 +16988,7 @@
         <v>0</v>
       </c>
       <c r="BO69">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="70" spans="1:67">
@@ -17134,7 +17134,7 @@
         <v>0</v>
       </c>
       <c r="BO70">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="71" spans="1:67">
@@ -17280,7 +17280,7 @@
         <v>1</v>
       </c>
       <c r="BO71">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="72" spans="1:67">
@@ -17429,7 +17429,7 @@
         <v>6</v>
       </c>
       <c r="BO72">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="73" spans="1:67">
@@ -17569,7 +17569,7 @@
         <v>4</v>
       </c>
       <c r="BO73">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="74" spans="1:67">
@@ -17724,7 +17724,7 @@
         <v>5</v>
       </c>
       <c r="BO74">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="75" spans="1:67">
@@ -17879,7 +17879,7 @@
         <v>1</v>
       </c>
       <c r="BO75">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="76" spans="1:67">
@@ -18016,7 +18016,7 @@
         <v>4</v>
       </c>
       <c r="BO76">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="77" spans="1:67">
@@ -18162,7 +18162,7 @@
         <v>2</v>
       </c>
       <c r="BO77">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="78" spans="1:67">
@@ -18302,7 +18302,7 @@
         <v>1</v>
       </c>
       <c r="BO78">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="79" spans="1:67">
@@ -18445,7 +18445,7 @@
         <v>0</v>
       </c>
       <c r="BO79">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="80" spans="1:67">
@@ -18603,7 +18603,7 @@
         <v>10</v>
       </c>
       <c r="BO80">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="81" spans="1:67">
@@ -18737,7 +18737,7 @@
         <v>8</v>
       </c>
       <c r="BO81">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="82" spans="1:67">
@@ -18889,7 +18889,7 @@
         <v>0</v>
       </c>
       <c r="BO82">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="83" spans="1:67">
@@ -19029,7 +19029,7 @@
         <v>1</v>
       </c>
       <c r="BO83">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="84" spans="1:67">
@@ -19172,7 +19172,7 @@
         <v>1</v>
       </c>
       <c r="BO84">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="85" spans="1:67">
@@ -19312,7 +19312,7 @@
         <v>7</v>
       </c>
       <c r="BO85">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="86" spans="1:67">
@@ -19452,7 +19452,7 @@
         <v>2</v>
       </c>
       <c r="BO86">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="87" spans="1:67">
@@ -19592,7 +19592,7 @@
         <v>4</v>
       </c>
       <c r="BO87">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="88" spans="1:67">
@@ -19738,7 +19738,7 @@
         <v>10</v>
       </c>
       <c r="BO88">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="89" spans="1:67">
@@ -19890,7 +19890,7 @@
         <v>4</v>
       </c>
       <c r="BO89">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="90" spans="1:67">
@@ -20021,7 +20021,7 @@
         <v>1</v>
       </c>
       <c r="BO90">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="91" spans="1:67">
@@ -20161,7 +20161,7 @@
         <v>10</v>
       </c>
       <c r="BO91">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="92" spans="1:67">
@@ -20295,7 +20295,7 @@
         <v>0</v>
       </c>
       <c r="BO92">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="93" spans="1:67">
@@ -20462,7 +20462,7 @@
         <v>5</v>
       </c>
       <c r="BO93">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="94" spans="1:67">
@@ -20614,7 +20614,7 @@
         <v>0</v>
       </c>
       <c r="BO94">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="95" spans="1:67">
@@ -20745,7 +20745,7 @@
         <v>0</v>
       </c>
       <c r="BO95">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="96" spans="1:67">
@@ -20873,7 +20873,7 @@
         <v>6</v>
       </c>
       <c r="BO96">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="97" spans="1:67">
@@ -21013,7 +21013,7 @@
         <v>1</v>
       </c>
       <c r="BO97">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="98" spans="1:67">
@@ -21156,7 +21156,7 @@
         <v>1</v>
       </c>
       <c r="BO98">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="99" spans="1:67">
@@ -21299,7 +21299,7 @@
         <v>0</v>
       </c>
       <c r="BO99">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="100" spans="1:67">
@@ -21448,7 +21448,7 @@
         <v>4</v>
       </c>
       <c r="BO100">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="101" spans="1:67">
@@ -21591,7 +21591,7 @@
         <v>0</v>
       </c>
       <c r="BO101">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="102" spans="1:67">
@@ -21737,7 +21737,7 @@
         <v>1</v>
       </c>
       <c r="BO102">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="103" spans="1:67">
@@ -21883,7 +21883,7 @@
         <v>1</v>
       </c>
       <c r="BO103">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="104" spans="1:67">
@@ -22026,7 +22026,7 @@
         <v>0</v>
       </c>
       <c r="BO104">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="105" spans="1:67">
@@ -22172,7 +22172,7 @@
         <v>0</v>
       </c>
       <c r="BO105">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="106" spans="1:67">
@@ -22312,7 +22312,7 @@
         <v>0</v>
       </c>
       <c r="BO106">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="107" spans="1:67">
@@ -22458,7 +22458,7 @@
         <v>8</v>
       </c>
       <c r="BO107">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="108" spans="1:67">
@@ -22613,7 +22613,7 @@
         <v>1</v>
       </c>
       <c r="BO108">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="109" spans="1:67">
@@ -22765,7 +22765,7 @@
         <v>3</v>
       </c>
       <c r="BO109">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="110" spans="1:67">
@@ -22905,7 +22905,7 @@
         <v>3</v>
       </c>
       <c r="BO110">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="111" spans="1:67">
@@ -23045,7 +23045,7 @@
         <v>1</v>
       </c>
       <c r="BO111">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="112" spans="1:67">
@@ -23167,7 +23167,7 @@
         <v>1</v>
       </c>
       <c r="BO112">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="113" spans="1:67">
@@ -23313,7 +23313,7 @@
         <v>0</v>
       </c>
       <c r="BO113">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="114" spans="1:67">
@@ -23459,7 +23459,7 @@
         <v>0</v>
       </c>
       <c r="BO114">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="115" spans="1:67">
@@ -23596,7 +23596,7 @@
         <v>1</v>
       </c>
       <c r="BO115">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="116" spans="1:67">
@@ -23748,7 +23748,7 @@
         <v>1</v>
       </c>
       <c r="BO116">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="117" spans="1:67">
@@ -23885,7 +23885,7 @@
         <v>1</v>
       </c>
       <c r="BO117">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="118" spans="1:67">
@@ -24037,7 +24037,7 @@
         <v>0</v>
       </c>
       <c r="BO118">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="119" spans="1:67">
@@ -24174,7 +24174,7 @@
         <v>7</v>
       </c>
       <c r="BO119">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="120" spans="1:67">
@@ -24305,7 +24305,7 @@
         <v>1</v>
       </c>
       <c r="BO120">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="121" spans="1:67">
@@ -24439,7 +24439,7 @@
         <v>1</v>
       </c>
       <c r="BO121">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="122" spans="1:67">
@@ -24564,7 +24564,7 @@
         <v>1</v>
       </c>
       <c r="BO122">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="123" spans="1:67">
@@ -24716,7 +24716,7 @@
         <v>1</v>
       </c>
       <c r="BO123">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="124" spans="1:67">
@@ -24868,7 +24868,7 @@
         <v>0</v>
       </c>
       <c r="BO124">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="125" spans="1:67">
@@ -25008,7 +25008,7 @@
         <v>1</v>
       </c>
       <c r="BO125">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="126" spans="1:67">
@@ -25157,7 +25157,7 @@
         <v>0</v>
       </c>
       <c r="BO126">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="127" spans="1:67">
@@ -25300,7 +25300,7 @@
         <v>1</v>
       </c>
       <c r="BO127">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="128" spans="1:67">
@@ -25437,7 +25437,7 @@
         <v>4</v>
       </c>
       <c r="BO128">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="129" spans="1:67">
@@ -25586,7 +25586,7 @@
         <v>1</v>
       </c>
       <c r="BO129">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="130" spans="1:67">
@@ -25723,7 +25723,7 @@
         <v>4</v>
       </c>
       <c r="BO130">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="131" spans="1:67">
@@ -25863,7 +25863,7 @@
         <v>8</v>
       </c>
       <c r="BO131">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="132" spans="1:67">
@@ -26000,7 +26000,7 @@
         <v>5</v>
       </c>
       <c r="BO132">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="133" spans="1:67">
@@ -26146,7 +26146,7 @@
         <v>2</v>
       </c>
       <c r="BO133">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="134" spans="1:67">
@@ -26289,7 +26289,7 @@
         <v>0</v>
       </c>
       <c r="BO134">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="135" spans="1:67">
@@ -26438,7 +26438,7 @@
         <v>5</v>
       </c>
       <c r="BO135">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="136" spans="1:67">
@@ -26590,7 +26590,7 @@
         <v>0</v>
       </c>
       <c r="BO136">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="137" spans="1:67">
@@ -26742,7 +26742,7 @@
         <v>5</v>
       </c>
       <c r="BO137">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="138" spans="1:67">
@@ -26867,7 +26867,7 @@
         <v>0</v>
       </c>
       <c r="BO138">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="139" spans="1:67">
@@ -27010,7 +27010,7 @@
         <v>3</v>
       </c>
       <c r="BO139">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="140" spans="1:67">
@@ -27150,7 +27150,7 @@
         <v>1</v>
       </c>
       <c r="BO140">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="141" spans="1:67">
@@ -27275,7 +27275,7 @@
         <v>0</v>
       </c>
       <c r="BO141">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="142" spans="1:67">
@@ -27415,7 +27415,7 @@
         <v>6</v>
       </c>
       <c r="BO142">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="143" spans="1:67">
@@ -27567,7 +27567,7 @@
         <v>0</v>
       </c>
       <c r="BO143">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="144" spans="1:67">
@@ -27704,7 +27704,7 @@
         <v>4</v>
       </c>
       <c r="BO144">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="145" spans="1:67">
@@ -27838,7 +27838,7 @@
         <v>0</v>
       </c>
       <c r="BO145">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="146" spans="1:67">
@@ -27996,7 +27996,7 @@
         <v>1</v>
       </c>
       <c r="BO146">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="147" spans="1:67">
@@ -28139,7 +28139,7 @@
         <v>0</v>
       </c>
       <c r="BO147">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="148" spans="1:67">
@@ -28261,7 +28261,7 @@
         <v>0</v>
       </c>
       <c r="BO148">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="149" spans="1:67">
@@ -28413,7 +28413,7 @@
         <v>5</v>
       </c>
       <c r="BO149">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="150" spans="1:67">
@@ -28559,7 +28559,7 @@
         <v>1</v>
       </c>
       <c r="BO150">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="151" spans="1:67">
@@ -28693,7 +28693,7 @@
         <v>7</v>
       </c>
       <c r="BO151">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="152" spans="1:67">
@@ -28842,7 +28842,7 @@
         <v>1</v>
       </c>
       <c r="BO152">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="153" spans="1:67">
@@ -28985,7 +28985,7 @@
         <v>1</v>
       </c>
       <c r="BO153">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="154" spans="1:67">
@@ -29122,7 +29122,7 @@
         <v>3</v>
       </c>
       <c r="BO154">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="155" spans="1:67">
@@ -29265,7 +29265,7 @@
         <v>3</v>
       </c>
       <c r="BO155">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="156" spans="1:67">
@@ -29399,7 +29399,7 @@
         <v>0</v>
       </c>
       <c r="BO156">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="157" spans="1:67">
@@ -29521,7 +29521,7 @@
         <v>0</v>
       </c>
       <c r="BO157">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="158" spans="1:67">
@@ -29661,7 +29661,7 @@
         <v>2</v>
       </c>
       <c r="BO158">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="159" spans="1:67">
@@ -29798,7 +29798,7 @@
         <v>0</v>
       </c>
       <c r="BO159">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="160" spans="1:67">
@@ -29950,7 +29950,7 @@
         <v>0</v>
       </c>
       <c r="BO160">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="161" spans="1:67">
@@ -30090,7 +30090,7 @@
         <v>3</v>
       </c>
       <c r="BO161">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="162" spans="1:67">
@@ -30230,7 +30230,7 @@
         <v>1</v>
       </c>
       <c r="BO162">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="163" spans="1:67">
@@ -30364,7 +30364,7 @@
         <v>1</v>
       </c>
       <c r="BO163">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="164" spans="1:67">
@@ -30516,7 +30516,7 @@
         <v>5</v>
       </c>
       <c r="BO164">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="165" spans="1:67">
@@ -30668,7 +30668,7 @@
         <v>1</v>
       </c>
       <c r="BO165">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="166" spans="1:67">
@@ -30808,7 +30808,7 @@
         <v>6</v>
       </c>
       <c r="BO166">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="167" spans="1:67">
@@ -30951,7 +30951,7 @@
         <v>0</v>
       </c>
       <c r="BO167">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="168" spans="1:67">
@@ -31097,7 +31097,7 @@
         <v>1</v>
       </c>
       <c r="BO168">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="169" spans="1:67">
@@ -31231,7 +31231,7 @@
         <v>0</v>
       </c>
       <c r="BO169">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="170" spans="1:67">
@@ -31377,7 +31377,7 @@
         <v>1</v>
       </c>
       <c r="BO170">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="171" spans="1:67">
@@ -31520,7 +31520,7 @@
         <v>1</v>
       </c>
       <c r="BO171">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="172" spans="1:67">
@@ -31681,7 +31681,7 @@
         <v>0</v>
       </c>
       <c r="BO172">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="173" spans="1:67">
@@ -31821,7 +31821,7 @@
         <v>1</v>
       </c>
       <c r="BO173">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="174" spans="1:67">
@@ -31943,7 +31943,7 @@
         <v>1</v>
       </c>
       <c r="BO174">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="175" spans="1:67">
@@ -32095,7 +32095,7 @@
         <v>0</v>
       </c>
       <c r="BO175">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="176" spans="1:67">
@@ -32238,7 +32238,7 @@
         <v>0</v>
       </c>
       <c r="BO176">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="177" spans="1:67">
@@ -32366,7 +32366,7 @@
         <v>1</v>
       </c>
       <c r="BO177">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="178" spans="1:67">
@@ -32515,7 +32515,7 @@
         <v>1</v>
       </c>
       <c r="BO178">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="179" spans="1:67">
@@ -32682,7 +32682,7 @@
         <v>12</v>
       </c>
       <c r="BO179">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="180" spans="1:67">
@@ -32813,7 +32813,7 @@
         <v>0</v>
       </c>
       <c r="BO180">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="181" spans="1:67">
@@ -32929,7 +32929,7 @@
         <v>1</v>
       </c>
       <c r="BO181">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="182" spans="1:67">
@@ -33084,7 +33084,7 @@
         <v>3</v>
       </c>
       <c r="BO182">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="183" spans="1:67">
@@ -33230,7 +33230,7 @@
         <v>8</v>
       </c>
       <c r="BO183">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="184" spans="1:67">
@@ -33373,7 +33373,7 @@
         <v>1</v>
       </c>
       <c r="BO184">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="185" spans="1:67">
@@ -33510,7 +33510,7 @@
         <v>0</v>
       </c>
       <c r="BO185">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="186" spans="1:67">
@@ -33641,7 +33641,7 @@
         <v>0</v>
       </c>
       <c r="BO186">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="187" spans="1:67">
@@ -33796,7 +33796,7 @@
         <v>0</v>
       </c>
       <c r="BO187">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="188" spans="1:67">
@@ -33936,7 +33936,7 @@
         <v>5</v>
       </c>
       <c r="BO188">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="189" spans="1:67">
@@ -34082,7 +34082,7 @@
         <v>0</v>
       </c>
       <c r="BO189">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="190" spans="1:67">
@@ -34225,7 +34225,7 @@
         <v>0</v>
       </c>
       <c r="BO190">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="191" spans="1:67">
@@ -34362,7 +34362,7 @@
         <v>1</v>
       </c>
       <c r="BO191">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="192" spans="1:67">
@@ -34511,7 +34511,7 @@
         <v>1</v>
       </c>
       <c r="BO192">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="193" spans="1:67">
@@ -34669,7 +34669,7 @@
         <v>0</v>
       </c>
       <c r="BO193">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="194" spans="1:67">
@@ -34827,7 +34827,7 @@
         <v>1</v>
       </c>
       <c r="BO194">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="195" spans="1:67">
@@ -34976,7 +34976,7 @@
         <v>1</v>
       </c>
       <c r="BO195">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
     <row r="196" spans="1:67">
@@ -35116,7 +35116,7 @@
         <v>1</v>
       </c>
       <c r="BO196">
-        <v>2010</v>
+        <v>2338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>